<commit_message>
updated review service seed data
</commit_message>
<xml_diff>
--- a/product-search-service/src/main/resources/product-search.xlsx
+++ b/product-search-service/src/main/resources/product-search.xlsx
@@ -1368,8 +1368,8 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>